<commit_message>
added dynamic rendering to student_details
</commit_message>
<xml_diff>
--- a/data/algorithms_attendance.xlsx
+++ b/data/algorithms_attendance.xlsx
@@ -470,13 +470,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>83.7</v>
+        <v>73.5</v>
       </c>
       <c r="D2" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
@@ -489,13 +489,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>64.2</v>
+        <v>92.7</v>
       </c>
       <c r="D3" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="n">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
@@ -508,13 +508,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>87.09999999999999</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>86.40000000000001</v>
+        <v>71</v>
       </c>
       <c r="D5" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E5" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>91.3</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>